<commit_message>
Dict changes inc. new German translations
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviaschmidt 1/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B23D14-0C9A-AE4D-BBDE-CCB094FF46CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA20A20-D3AC-034B-A7AA-3C7BFED87F5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
+    <workbookView xWindow="180" yWindow="1140" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add flute to allowed instruments and factor instrument list stuff
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviaschmidt 1/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA20A20-D3AC-034B-A7AA-3C7BFED87F5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB3FF61-9E84-6F41-BFA9-8517DB385BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1140" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
+    <workbookView xWindow="13120" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Piano</t>
   </si>
@@ -145,6 +145,33 @@
   </si>
   <si>
     <t>auto</t>
+  </si>
+  <si>
+    <t>Bass Clarinet</t>
+  </si>
+  <si>
+    <t>Cornet</t>
+  </si>
+  <si>
+    <t>C Tenor Saxophone</t>
+  </si>
+  <si>
+    <t>bass_clarinet</t>
+  </si>
+  <si>
+    <t>cornet</t>
+  </si>
+  <si>
+    <t>c_tenor_saxophone</t>
+  </si>
+  <si>
+    <t>Bassklarinette</t>
+  </si>
+  <si>
+    <t>Kornett</t>
+  </si>
+  <si>
+    <t>C-Tenor Saxophon</t>
   </si>
 </sst>
 </file>
@@ -527,7 +554,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,8 +795,74 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2">
+        <v>84</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2">
+        <v>76</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>

</xml_diff>

<commit_message>
Updated Latvian and German translations
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18355BE1-1BB1-7B4D-BD6D-5B90CCD23083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA5FB1-399E-2D43-95DC-A2810FFF805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Piano</t>
   </si>
@@ -175,13 +175,61 @@
   </si>
   <si>
     <t>it</t>
+  </si>
+  <si>
+    <t>voice</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>Stimme</t>
+  </si>
+  <si>
+    <t>Klavieres</t>
+  </si>
+  <si>
+    <t>Flauta</t>
+  </si>
+  <si>
+    <t>Klarnete</t>
+  </si>
+  <si>
+    <t>Soprāna saksofons</t>
+  </si>
+  <si>
+    <t>Alta saksofons</t>
+  </si>
+  <si>
+    <t>Tenora saksofons</t>
+  </si>
+  <si>
+    <t>Baritona saksofons</t>
+  </si>
+  <si>
+    <t>Trombons</t>
+  </si>
+  <si>
+    <t>Basa klarnete</t>
+  </si>
+  <si>
+    <t>Kornete</t>
+  </si>
+  <si>
+    <t>C - tenora saksofons</t>
+  </si>
+  <si>
+    <t>Balss</t>
+  </si>
+  <si>
+    <t>lv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -213,6 +261,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,12 +289,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFE8AF5-2A59-E340-94E0-F3103F65052D}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="E3" sqref="E3:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +625,7 @@
     <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -582,337 +639,403 @@
         <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="2">
+        <v>48</v>
+      </c>
+      <c r="G2" s="2">
+        <v>72</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2">
         <v>45</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G3" s="2">
         <v>81</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1">
         <v>60</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G4" s="2">
         <v>96</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1">
         <v>50</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G5" s="2">
         <v>94</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H5" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="1">
         <v>56</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G6" s="2">
         <v>88</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1">
         <v>49</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G7" s="2">
         <v>81</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H7" s="2">
         <v>-3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="1">
         <v>44</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>76</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H8" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2">
         <v>36</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>69</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-3</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1">
         <v>55</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>82</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>2</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
         <v>40</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>72</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2">
         <v>34</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>83</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>2</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2">
         <v>54</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>84</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>2</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="2">
         <v>44</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>76</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -929,6 +1052,9 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Large update to support MySQL DB usage and "paradigm" feature
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA5FB1-399E-2D43-95DC-A2810FFF805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C753E-908A-ED4A-89A6-49D16A540711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -289,14 +289,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +613,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,7 +850,7 @@
         <v>76</v>
       </c>
       <c r="H8" s="2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>34</v>
@@ -1033,7 +1032,6 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>

</xml_diff>

<commit_message>
Add support for string instruments
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C753E-908A-ED4A-89A6-49D16A540711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F07AE60-1680-AE49-BCEC-60C12C93EEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>Piano</t>
   </si>
@@ -223,6 +223,33 @@
   </si>
   <si>
     <t>lv</t>
+  </si>
+  <si>
+    <t>violin</t>
+  </si>
+  <si>
+    <t>viola</t>
+  </si>
+  <si>
+    <t>cello</t>
+  </si>
+  <si>
+    <t>double_bass</t>
+  </si>
+  <si>
+    <t>Violin</t>
+  </si>
+  <si>
+    <t>Viola</t>
+  </si>
+  <si>
+    <t>Cello</t>
+  </si>
+  <si>
+    <t>Double Bass</t>
+  </si>
+  <si>
+    <t>alto</t>
   </si>
 </sst>
 </file>
@@ -314,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -460,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,7 +640,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,27 +1058,131 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2">
+        <v>55</v>
+      </c>
+      <c r="G15" s="2">
+        <v>93</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2">
+        <v>48</v>
+      </c>
+      <c r="G16" s="2">
+        <v>84</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2">
+        <v>84</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2">
+        <v>67</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixing across project merges
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C753E-908A-ED4A-89A6-49D16A540711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F07AE60-1680-AE49-BCEC-60C12C93EEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="500" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>Piano</t>
   </si>
@@ -223,6 +223,33 @@
   </si>
   <si>
     <t>lv</t>
+  </si>
+  <si>
+    <t>violin</t>
+  </si>
+  <si>
+    <t>viola</t>
+  </si>
+  <si>
+    <t>cello</t>
+  </si>
+  <si>
+    <t>double_bass</t>
+  </si>
+  <si>
+    <t>Violin</t>
+  </si>
+  <si>
+    <t>Viola</t>
+  </si>
+  <si>
+    <t>Cello</t>
+  </si>
+  <si>
+    <t>Double Bass</t>
+  </si>
+  <si>
+    <t>alto</t>
   </si>
 </sst>
 </file>
@@ -314,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -460,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,7 +640,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,27 +1058,131 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2">
+        <v>55</v>
+      </c>
+      <c r="G15" s="2">
+        <v>93</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2">
+        <v>48</v>
+      </c>
+      <c r="G16" s="2">
+        <v>84</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2">
+        <v>84</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2">
+        <v>67</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Electric Bass to instruments
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994729F1-6EA9-E649-8C2D-F01DDDD889BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDADE7DA-8387-A44F-A7AE-0A11E63919DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="920" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
+    <workbookView xWindow="3080" yWindow="1180" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
   <si>
     <t>Piano</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Electric Bass</t>
+  </si>
+  <si>
+    <t>E-Bass</t>
+  </si>
+  <si>
+    <t>electric_bass</t>
   </si>
 </sst>
 </file>
@@ -295,11 +304,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -645,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFE8AF5-2A59-E340-94E0-F3103F65052D}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,34 +669,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -736,7 +745,7 @@
       <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F3" s="2">
@@ -768,7 +777,7 @@
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="1">
@@ -800,7 +809,7 @@
       <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="1">
@@ -832,7 +841,7 @@
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="1">
@@ -864,7 +873,7 @@
       <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="1">
@@ -896,7 +905,7 @@
       <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="1">
@@ -928,7 +937,7 @@
       <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F9" s="2">
@@ -960,7 +969,7 @@
       <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="1">
@@ -992,7 +1001,7 @@
       <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="1">
@@ -1024,7 +1033,7 @@
       <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F12" s="2">
@@ -1056,7 +1065,7 @@
       <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F13" s="2">
@@ -1076,7 +1085,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1088,7 +1097,7 @@
       <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="2">
@@ -1108,7 +1117,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1140,7 +1149,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1172,7 +1181,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1204,7 +1213,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1226,7 +1235,7 @@
         <v>67</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>35</v>
@@ -1236,7 +1245,36 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="2">
+        <v>28</v>
+      </c>
+      <c r="G19" s="2">
+        <v>67</v>
+      </c>
+      <c r="H19" s="2">
+        <v>12</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>

</xml_diff>

<commit_message>
Add Drums to musical instrument selector
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25063443-2A42-8941-9DD7-98F911CAD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E7FD1-1007-404A-A688-374E336FE511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="1180" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>Piano</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>Rhythmus</t>
+  </si>
+  <si>
+    <t>drums</t>
+  </si>
+  <si>
+    <t>Drums</t>
+  </si>
+  <si>
+    <t>Schlagzeug</t>
   </si>
 </sst>
 </file>
@@ -664,7 +673,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,7 +1327,36 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>99</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>

</xml_diff>

<commit_message>
Add transposition for highest_reading_note
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E7FD1-1007-404A-A688-374E336FE511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018DAFFD-333B-BE4D-89D9-486E53E0CE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="1180" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
+    <workbookView xWindow="1300" yWindow="1280" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>Piano</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Schlagzeug</t>
+  </si>
+  <si>
+    <t>highest_reading_note</t>
   </si>
 </sst>
 </file>
@@ -670,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFE8AF5-2A59-E340-94E0-F3103F65052D}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,10 +686,11 @@
     <col min="3" max="3" width="31.1640625" style="2" customWidth="1"/>
     <col min="4" max="9" width="10.83203125" style="2"/>
     <col min="10" max="10" width="25.5" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="39.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -717,8 +721,11 @@
       <c r="J1" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -749,8 +756,11 @@
       <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -781,8 +791,11 @@
       <c r="J3" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -813,8 +826,11 @@
       <c r="J4" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -845,8 +861,11 @@
       <c r="J5" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -877,8 +896,11 @@
       <c r="J6" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -909,8 +931,11 @@
       <c r="J7" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -941,8 +966,11 @@
       <c r="J8" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -973,8 +1001,11 @@
       <c r="J9" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1005,8 +1036,11 @@
       <c r="J10" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1037,8 +1071,11 @@
       <c r="J11" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
@@ -1069,8 +1106,11 @@
       <c r="J12" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -1101,8 +1141,11 @@
       <c r="J13" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1133,8 +1176,11 @@
       <c r="J14" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>63</v>
       </c>
@@ -1165,8 +1211,11 @@
       <c r="J15" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>64</v>
       </c>
@@ -1197,8 +1246,11 @@
       <c r="J16" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>65</v>
       </c>
@@ -1229,8 +1281,11 @@
       <c r="J17" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>66</v>
       </c>
@@ -1261,8 +1316,11 @@
       <c r="J18" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>77</v>
       </c>
@@ -1293,8 +1351,11 @@
       <c r="J19" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>76</v>
       </c>
@@ -1325,8 +1386,11 @@
       <c r="J20" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>80</v>
       </c>
@@ -1357,11 +1421,14 @@
       <c r="J21" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Acoustic and Electric guitar to instruments
</commit_message>
<xml_diff>
--- a/data-raw/musical_instruments.xlsx
+++ b/data-raw/musical_instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/musicassessr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018DAFFD-333B-BE4D-89D9-486E53E0CE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E38AD59-6280-5449-B65E-7C8AFD71E6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="1280" windowWidth="27640" windowHeight="16860" xr2:uid="{CB7537FB-C9CF-C142-AE58-74683695060A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
   <si>
     <t>Piano</t>
   </si>
@@ -286,6 +286,36 @@
   </si>
   <si>
     <t>highest_reading_note</t>
+  </si>
+  <si>
+    <t>acoustic_guitar</t>
+  </si>
+  <si>
+    <t>Acoustic Guitar</t>
+  </si>
+  <si>
+    <t>Chitarra Acustica</t>
+  </si>
+  <si>
+    <t>Akustikgitarre</t>
+  </si>
+  <si>
+    <t>Akustiskā ģitāra</t>
+  </si>
+  <si>
+    <t>electric_guitar</t>
+  </si>
+  <si>
+    <t>Electric Guitar</t>
+  </si>
+  <si>
+    <t>Chitarra Elettrica</t>
+  </si>
+  <si>
+    <t>E-Gitarre</t>
+  </si>
+  <si>
+    <t>Elektriskā ģitāra</t>
   </si>
 </sst>
 </file>
@@ -676,7 +706,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A22" sqref="A22:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,10 +1456,74 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
+      </c>
+      <c r="G22">
+        <v>88</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22">
+        <v>40</v>
+      </c>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23">
+        <v>88</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23">
+        <v>40</v>
+      </c>
+      <c r="K23" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>